<commit_message>
Eliminadas tablas de Venias
</commit_message>
<xml_diff>
--- a/uploads/database.xlsx
+++ b/uploads/database.xlsx
@@ -6476,14 +6476,26 @@
           <t>1</t>
         </is>
       </c>
-      <c r="G153" t="inlineStr"/>
-      <c r="H153" t="inlineStr"/>
+      <c r="G153" t="inlineStr">
+        <is>
+          <t>2222</t>
+        </is>
+      </c>
+      <c r="H153" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
       <c r="I153" t="inlineStr">
         <is>
           <t>570</t>
         </is>
       </c>
-      <c r="J153" t="inlineStr"/>
+      <c r="J153" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
@@ -6516,26 +6528,14 @@
           <t>2</t>
         </is>
       </c>
-      <c r="G154" t="inlineStr">
-        <is>
-          <t>3333</t>
-        </is>
-      </c>
-      <c r="H154" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
-      </c>
+      <c r="G154" t="inlineStr"/>
+      <c r="H154" t="inlineStr"/>
       <c r="I154" t="inlineStr">
         <is>
           <t>570</t>
         </is>
       </c>
-      <c r="J154" t="inlineStr">
-        <is>
-          <t>Sí</t>
-        </is>
-      </c>
+      <c r="J154" t="inlineStr"/>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
@@ -6568,26 +6568,14 @@
           <t>41</t>
         </is>
       </c>
-      <c r="G155" t="inlineStr">
-        <is>
-          <t>3333</t>
-        </is>
-      </c>
-      <c r="H155" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
-      </c>
+      <c r="G155" t="inlineStr"/>
+      <c r="H155" t="inlineStr"/>
       <c r="I155" t="inlineStr">
         <is>
           <t>570</t>
         </is>
       </c>
-      <c r="J155" t="inlineStr">
-        <is>
-          <t>Sí</t>
-        </is>
-      </c>
+      <c r="J155" t="inlineStr"/>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
@@ -6620,26 +6608,14 @@
           <t>42</t>
         </is>
       </c>
-      <c r="G156" t="inlineStr">
-        <is>
-          <t>3333</t>
-        </is>
-      </c>
-      <c r="H156" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
-      </c>
+      <c r="G156" t="inlineStr"/>
+      <c r="H156" t="inlineStr"/>
       <c r="I156" t="inlineStr">
         <is>
           <t>570</t>
         </is>
       </c>
-      <c r="J156" t="inlineStr">
-        <is>
-          <t>Sí</t>
-        </is>
-      </c>
+      <c r="J156" t="inlineStr"/>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
@@ -12644,26 +12620,14 @@
           <t>17</t>
         </is>
       </c>
-      <c r="G306" t="inlineStr">
-        <is>
-          <t>3333</t>
-        </is>
-      </c>
-      <c r="H306" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
+      <c r="G306" t="inlineStr"/>
+      <c r="H306" t="inlineStr"/>
       <c r="I306" t="inlineStr">
         <is>
           <t>35</t>
         </is>
       </c>
-      <c r="J306" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="J306" t="inlineStr"/>
     </row>
     <row r="307">
       <c r="A307" t="inlineStr">
@@ -12696,26 +12660,14 @@
           <t>41</t>
         </is>
       </c>
-      <c r="G307" t="inlineStr">
-        <is>
-          <t>3333</t>
-        </is>
-      </c>
-      <c r="H307" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
+      <c r="G307" t="inlineStr"/>
+      <c r="H307" t="inlineStr"/>
       <c r="I307" t="inlineStr">
         <is>
           <t>35</t>
         </is>
       </c>
-      <c r="J307" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="J307" t="inlineStr"/>
     </row>
     <row r="308">
       <c r="A308" t="inlineStr">

</xml_diff>